<commit_message>
interim voltage upgrade changes
</commit_message>
<xml_diff>
--- a/disco/extensions/upgrade_simulation/upgrades/Generic_DISCO_cost_database_v2.xlsx
+++ b/disco/extensions/upgrade_simulation/upgrades/Generic_DISCO_cost_database_v2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SABRAHAM\Documents\GitHub\Tools\disco\disco\extensions\upgrade_simulation\upgrades\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6EEFA48-40DD-4E67-9A40-68920FF48FE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4F1E7FA-6338-49BF-BD12-09A96A709579}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="676" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-57720" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="676" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="lines" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="754" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="762" uniqueCount="38">
   <si>
     <t>cost_per_m</t>
   </si>
@@ -100,19 +100,10 @@
     <t>Assume that the costs for each row are inclusive of labor/land/etc. User has to ensure that.</t>
   </si>
   <si>
-    <t>Change LTC setpoint</t>
-  </si>
-  <si>
     <t>Replace voltage regulator controller</t>
   </si>
   <si>
-    <t>Change LTC controller</t>
-  </si>
-  <si>
     <t>Type</t>
-  </si>
-  <si>
-    <t>Add new voltage regulator</t>
   </si>
   <si>
     <t>Replace capacitor controller</t>
@@ -125,9 +116,6 @@
   </si>
   <si>
     <t>secondary_kV</t>
-  </si>
-  <si>
-    <t>transformer_kVA</t>
   </si>
   <si>
     <t>voltage_kV</t>
@@ -152,6 +140,15 @@
   </si>
   <si>
     <t>If new transformer is added in parallel, then removing and replacing fixed costs are considered (refer sheet misc)</t>
+  </si>
+  <si>
+    <t>Add new voltage regulator transformer</t>
+  </si>
+  <si>
+    <t>Add new LTC controller</t>
+  </si>
+  <si>
+    <t>Change LTC settings</t>
   </si>
 </sst>
 </file>
@@ -306,7 +303,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -484,6 +481,12 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -668,7 +671,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -694,6 +697,8 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="166" fontId="0" fillId="33" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="20" builtinId="30" customBuiltin="1"/>
@@ -1068,13 +1073,13 @@
   <sheetData>
     <row r="1" spans="1:9" s="9" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>27</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>31</v>
       </c>
       <c r="D1" s="7" t="s">
         <v>9</v>
@@ -4046,7 +4051,7 @@
   <dimension ref="A1:I106"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4065,10 +4070,10 @@
         <v>2</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D1" s="7" t="s">
         <v>18</v>
@@ -7144,7 +7149,7 @@
   <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="A5" sqref="A5:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -7154,7 +7159,7 @@
   <sheetData>
     <row r="1" spans="1:9" s="9" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B1" s="7" t="s">
         <v>16</v>
@@ -7171,7 +7176,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>37</v>
       </c>
       <c r="B2" s="4">
         <v>500</v>
@@ -7181,10 +7186,10 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B3" s="4">
+      <c r="A3" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" s="14">
         <v>15000</v>
       </c>
       <c r="C3" t="s">
@@ -7193,7 +7198,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B4" s="4">
         <v>500</v>
@@ -7204,20 +7209,19 @@
       <c r="D4" s="3"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>36</v>
-      </c>
-      <c r="B5" s="4">
-        <v>2000</v>
+      <c r="A5" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" s="14">
+        <v>15000</v>
       </c>
       <c r="C5" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="3"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B6" s="4">
         <v>3500</v>
@@ -7228,21 +7232,22 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="B7" s="4">
-        <v>3500</v>
+        <v>2000</v>
       </c>
       <c r="C7" t="s">
         <v>1</v>
       </c>
+      <c r="D7" s="3"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="B8" s="4">
-        <v>0</v>
+        <v>3500</v>
       </c>
       <c r="C8" t="s">
         <v>1</v>
@@ -7250,10 +7255,10 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B9" s="4">
-        <v>15000</v>
+        <v>0</v>
       </c>
       <c r="C9" t="s">
         <v>1</v>
@@ -7275,88 +7280,121 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.75" customWidth="1"/>
+    <col min="1" max="1" width="32.875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.875" customWidth="1"/>
     <col min="3" max="3" width="17.25" style="5" customWidth="1"/>
     <col min="4" max="4" width="12.625" customWidth="1"/>
     <col min="5" max="5" width="11.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="9" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="9" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B1" s="7" t="s">
         <v>2</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="E1" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="J1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="8"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="5">
+        <v>3</v>
+      </c>
+      <c r="C2" s="5">
         <v>25</v>
-      </c>
-      <c r="B2" s="5">
-        <v>3</v>
-      </c>
-      <c r="C2" s="5">
-        <v>10000</v>
       </c>
       <c r="D2" s="5">
         <v>25</v>
       </c>
       <c r="E2" s="5">
+        <v>2</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" s="5">
+        <v>10000</v>
+      </c>
+      <c r="I2" s="5">
         <v>220000</v>
       </c>
-      <c r="F2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="B3" s="5">
         <v>3</v>
       </c>
       <c r="C3" s="5">
+        <v>12.47</v>
+      </c>
+      <c r="D3" s="5">
+        <v>12.47</v>
+      </c>
+      <c r="E3" s="5">
+        <v>2</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" s="5">
         <v>10000</v>
       </c>
-      <c r="D3" s="5">
-        <v>12.47</v>
-      </c>
-      <c r="E3" s="5">
+      <c r="I3" s="5">
         <v>150000</v>
       </c>
-      <c r="F3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E4" s="4"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E5" s="4"/>
     </row>
   </sheetData>
@@ -7368,7 +7406,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{403E8DB1-5F2A-4BA6-B37A-04170EF10F2B}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
@@ -7379,7 +7417,7 @@
   <sheetData>
     <row r="1" spans="1:3" s="12" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B1" s="11" t="s">
         <v>4</v>
@@ -7390,7 +7428,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B2" s="4">
         <v>0</v>
@@ -7401,7 +7439,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B3" s="4">
         <v>0</v>
@@ -7458,7 +7496,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add jsonencoder, fix costdatabase field
</commit_message>
<xml_diff>
--- a/disco/extensions/upgrade_simulation/upgrades/Generic_DISCO_cost_database_v2.xlsx
+++ b/disco/extensions/upgrade_simulation/upgrades/Generic_DISCO_cost_database_v2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SABRAHAM\Documents\GitHub\Tools\disco\disco\extensions\upgrade_simulation\upgrades\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33C5616E-ABE0-48E0-BC2A-85B7CEA39721}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9321B5AE-938E-43FC-8ACC-A16C7693C197}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12720" tabRatio="676" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="676" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="lines" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="762" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="762" uniqueCount="39">
   <si>
     <t>cost_per_m</t>
   </si>
@@ -149,6 +149,9 @@
   </si>
   <si>
     <t>description</t>
+  </si>
+  <si>
+    <t>upgrade_type</t>
   </si>
 </sst>
 </file>
@@ -1057,8 +1060,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I129"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1073,7 +1076,7 @@
   <sheetData>
     <row r="1" spans="1:9" s="9" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B1" s="7" t="s">
         <v>2</v>
@@ -7465,7 +7468,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5E97FA0-EA86-42FF-9B53-994C6673BFB4}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>

</xml_diff>